<commit_message>
BME xlsx push off the pi
</commit_message>
<xml_diff>
--- a/climate.xlsx
+++ b/climate.xlsx
@@ -7,12 +7,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Humidity" localSheetId="0">'Sheet1'!$A$2:$A$196</definedName>
+    <definedName name="temp" localSheetId="0">'Sheet1'!$B$2:$B$196</definedName>
+    <definedName name="gas" localSheetId="0">'Sheet1'!$C$2:$C$196</definedName>
+    <definedName name="farenheit" localSheetId="0">'Sheet1'!$D$2:$D$196</definedName>
+    <definedName name="centigrade" localSheetId="0">'Sheet1'!$E$2:$E$196</definedName>
+    <definedName name="time" localSheetId="0">'Sheet1'!$F$2:$F$196</definedName>
+  </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>Humidity</t>
   </si>
@@ -567,6 +575,54 @@
   </si>
   <si>
     <t>Fri, 27 May 2022 05:22:22 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:23:29 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:24:38 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:25:43 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:26:51 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:27:57 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:29:06 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:30:10 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:31:20 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:32:28 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:33:37 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:34:46 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:35:54 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:37:03 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:38:12 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:39:21 GMT</t>
+  </si>
+  <si>
+    <t>Fri, 27 May 2022 05:40:30 GMT</t>
   </si>
 </sst>
 </file>
@@ -610,9 +666,143 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>temp over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Series 1</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sheet1'!time</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1'!farenheit</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:overlap val="100"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="ChartA2beXI"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F180"/>
+  <dimension ref="A1:F196"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4218,7 +4408,328 @@
         <v>184</v>
       </c>
     </row>
+    <row r="181">
+      <c r="A181" s="0">
+        <v>54.56</v>
+      </c>
+      <c r="B181" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="C181" s="0">
+        <v>272.85</v>
+      </c>
+      <c r="D181" s="0">
+        <v>78.836</v>
+      </c>
+      <c r="E181" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="F181" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="0">
+        <v>54.17</v>
+      </c>
+      <c r="B182" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="C182" s="0">
+        <v>274.44</v>
+      </c>
+      <c r="D182" s="0">
+        <v>78.836</v>
+      </c>
+      <c r="E182" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="F182" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0">
+        <v>54.18</v>
+      </c>
+      <c r="B183" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="C183" s="0">
+        <v>276.5</v>
+      </c>
+      <c r="D183" s="0">
+        <v>78.836</v>
+      </c>
+      <c r="E183" s="0">
+        <v>26.02</v>
+      </c>
+      <c r="F183" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="0">
+        <v>53.92</v>
+      </c>
+      <c r="B184" s="0">
+        <v>26</v>
+      </c>
+      <c r="C184" s="0">
+        <v>275.35</v>
+      </c>
+      <c r="D184" s="0">
+        <v>78.8</v>
+      </c>
+      <c r="E184" s="0">
+        <v>26</v>
+      </c>
+      <c r="F184" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0">
+        <v>53.92</v>
+      </c>
+      <c r="B185" s="0">
+        <v>25.99</v>
+      </c>
+      <c r="C185" s="0">
+        <v>277.2</v>
+      </c>
+      <c r="D185" s="0">
+        <v>78.782</v>
+      </c>
+      <c r="E185" s="0">
+        <v>25.99</v>
+      </c>
+      <c r="F185" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="0">
+        <v>53.96</v>
+      </c>
+      <c r="B186" s="0">
+        <v>25.98</v>
+      </c>
+      <c r="C186" s="0">
+        <v>275.81</v>
+      </c>
+      <c r="D186" s="0">
+        <v>78.764</v>
+      </c>
+      <c r="E186" s="0">
+        <v>25.98</v>
+      </c>
+      <c r="F186" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="0">
+        <v>53.9</v>
+      </c>
+      <c r="B187" s="0">
+        <v>25.94</v>
+      </c>
+      <c r="C187" s="0">
+        <v>276.97</v>
+      </c>
+      <c r="D187" s="0">
+        <v>78.69200000000001</v>
+      </c>
+      <c r="E187" s="0">
+        <v>25.94</v>
+      </c>
+      <c r="F187" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="0">
+        <v>53.97</v>
+      </c>
+      <c r="B188" s="0">
+        <v>25.91</v>
+      </c>
+      <c r="C188" s="0">
+        <v>277.66</v>
+      </c>
+      <c r="D188" s="0">
+        <v>78.638</v>
+      </c>
+      <c r="E188" s="0">
+        <v>25.91</v>
+      </c>
+      <c r="F188" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="0">
+        <v>54.03</v>
+      </c>
+      <c r="B189" s="0">
+        <v>25.86</v>
+      </c>
+      <c r="C189" s="0">
+        <v>278.37</v>
+      </c>
+      <c r="D189" s="0">
+        <v>78.548</v>
+      </c>
+      <c r="E189" s="0">
+        <v>25.86</v>
+      </c>
+      <c r="F189" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="0">
+        <v>54.44</v>
+      </c>
+      <c r="B190" s="0">
+        <v>25.8</v>
+      </c>
+      <c r="C190" s="0">
+        <v>277.9</v>
+      </c>
+      <c r="D190" s="0">
+        <v>78.44</v>
+      </c>
+      <c r="E190" s="0">
+        <v>25.8</v>
+      </c>
+      <c r="F190" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0">
+        <v>54.52</v>
+      </c>
+      <c r="B191" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="C191" s="0">
+        <v>277.66</v>
+      </c>
+      <c r="D191" s="0">
+        <v>78.35</v>
+      </c>
+      <c r="E191" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="F191" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="0">
+        <v>54.78</v>
+      </c>
+      <c r="B192" s="0">
+        <v>25.78</v>
+      </c>
+      <c r="C192" s="0">
+        <v>277.2</v>
+      </c>
+      <c r="D192" s="0">
+        <v>78.404</v>
+      </c>
+      <c r="E192" s="0">
+        <v>25.78</v>
+      </c>
+      <c r="F192" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="0">
+        <v>55.78</v>
+      </c>
+      <c r="B193" s="0">
+        <v>25.83</v>
+      </c>
+      <c r="C193" s="0">
+        <v>274.89</v>
+      </c>
+      <c r="D193" s="0">
+        <v>78.494</v>
+      </c>
+      <c r="E193" s="0">
+        <v>25.83</v>
+      </c>
+      <c r="F193" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="0">
+        <v>55.11</v>
+      </c>
+      <c r="B194" s="0">
+        <v>25.84</v>
+      </c>
+      <c r="C194" s="0">
+        <v>275.81</v>
+      </c>
+      <c r="D194" s="0">
+        <v>78.512</v>
+      </c>
+      <c r="E194" s="0">
+        <v>25.84</v>
+      </c>
+      <c r="F194" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="0">
+        <v>55.19</v>
+      </c>
+      <c r="B195" s="0">
+        <v>25.78</v>
+      </c>
+      <c r="C195" s="0">
+        <v>275.35</v>
+      </c>
+      <c r="D195" s="0">
+        <v>78.404</v>
+      </c>
+      <c r="E195" s="0">
+        <v>25.78</v>
+      </c>
+      <c r="F195" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="0">
+        <v>55.19</v>
+      </c>
+      <c r="B196" s="0">
+        <v>25.82</v>
+      </c>
+      <c r="C196" s="0">
+        <v>276.27</v>
+      </c>
+      <c r="D196" s="0">
+        <v>78.476</v>
+      </c>
+      <c r="E196" s="0">
+        <v>25.82</v>
+      </c>
+      <c r="F196" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>